<commit_message>
Added LiPo Fuel Gauges
these were the only ones i could find
</commit_message>
<xml_diff>
--- a/Documentation/Budget/Parts Order.xlsx
+++ b/Documentation/Budget/Parts Order.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bpowe_000\Documents\GitHub\CapStone\Documentation\Budget\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Documents\GitHub\CapStone\Documentation\Budget\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Item</t>
   </si>
@@ -117,6 +117,12 @@
   </si>
   <si>
     <t>https://www.sparkfun.com/products/9454</t>
+  </si>
+  <si>
+    <t>LiPo Fuel Gauge</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/10617</t>
   </si>
 </sst>
 </file>
@@ -166,17 +172,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="8" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="8" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -457,15 +463,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H11"/>
+  <dimension ref="A2:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -488,7 +494,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -512,7 +518,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -532,18 +538,18 @@
         <v>11.72</v>
       </c>
       <c r="G4" s="2">
-        <f t="shared" ref="G4:G11" si="0">D4*E4+F4</f>
+        <f t="shared" ref="G4:G12" si="0">D4*E4+F4</f>
         <v>71.710000000000008</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
       <c r="B5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D5" s="2">
@@ -552,7 +558,7 @@
       <c r="E5">
         <v>1</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="6">
         <v>0</v>
       </c>
       <c r="G5" s="2">
@@ -560,47 +566,47 @@
         <v>13.99</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
       <c r="B6" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="4"/>
+      <c r="C6" s="5"/>
       <c r="D6" s="2">
         <v>7.99</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
-      <c r="F6" s="3"/>
+      <c r="F6" s="7"/>
       <c r="G6" s="2">
         <f t="shared" si="0"/>
         <v>7.99</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
       <c r="B7" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="4"/>
+      <c r="C7" s="5"/>
       <c r="D7" s="2">
         <v>79.430000000000007</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
-      <c r="F7" s="3"/>
+      <c r="F7" s="7"/>
       <c r="G7" s="2">
         <f t="shared" si="0"/>
         <v>79.430000000000007</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -624,38 +630,38 @@
         <v>149</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="6" t="s">
+    <row r="9" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="4">
         <v>12.95</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="3">
         <v>3</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="4">
         <f t="shared" si="0"/>
         <v>38.849999999999994</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="H9" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>28</v>
       </c>
       <c r="B10" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="4"/>
+      <c r="C10" s="5"/>
       <c r="D10" s="2">
         <v>16.95</v>
       </c>
@@ -667,14 +673,14 @@
         <v>67.8</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>29</v>
       </c>
       <c r="B11" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="4"/>
+      <c r="C11" s="5"/>
       <c r="D11" s="2">
         <v>2.95</v>
       </c>
@@ -684,13 +690,32 @@
       <c r="G11" s="2">
         <f t="shared" si="0"/>
         <v>14.75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="2">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="G12" s="2">
+        <f t="shared" si="0"/>
+        <v>19.899999999999999</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="C5:C7"/>
     <mergeCell ref="F5:F7"/>
-    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C9:C12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>